<commit_message>
pass data from qty monitoring to follow up
</commit_message>
<xml_diff>
--- a/forms/app/quality_monitoring.xlsx
+++ b/forms/app/quality_monitoring.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="312">
   <si>
     <t>type</t>
   </si>
@@ -1005,6 +1005,9 @@
     <t>default_language</t>
   </si>
   <si>
+    <t>style</t>
+  </si>
+  <si>
     <t>quality_monitoring</t>
   </si>
   <si>
@@ -1012,6 +1015,9 @@
   </si>
   <si>
     <t>English (en)</t>
+  </si>
+  <si>
+    <t>pages</t>
   </si>
 </sst>
 </file>
@@ -30597,7 +30603,9 @@
       <c r="E1" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="F1" s="2"/>
+      <c r="F1" s="1" t="s">
+        <v>307</v>
+      </c>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
@@ -30624,19 +30632,21 @@
         <v>212</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C2" s="17">
         <f>NOW()</f>
-        <v>44732.48535</v>
+        <v>44741.60844</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
-      <c r="F2" s="4"/>
+      <c r="F2" s="3" t="s">
+        <v>311</v>
+      </c>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>

</xml_diff>

<commit_message>
add validation and summary pages
</commit_message>
<xml_diff>
--- a/forms/app/quality_monitoring.xlsx
+++ b/forms/app/quality_monitoring.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="326">
   <si>
     <t>type</t>
   </si>
@@ -864,16 +864,29 @@
     <t>field-list summary</t>
   </si>
   <si>
+    <t>r_chw_info_title</t>
+  </si>
+  <si>
+    <t>CHW Details &lt;i class="fa fa-user"&gt;&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>h2 blue</t>
+  </si>
+  <si>
     <t>r_chw_info</t>
   </si>
   <si>
-    <t>**${chw_name}** ID: ${chw_id}</t>
+    <t>&lt;div style="text-align:center;"&gt;&lt;span&gt;**CHV name:** ${chw_name}&lt;/span&gt; 
+&lt;span&gt;**CHV ID:** ${chw_id}&lt;/span&gt;&lt;/div&gt;</t>
   </si>
   <si>
     <t>r_improvement_areas_title</t>
   </si>
   <si>
     <t>Areas of Improvement &lt;i class="fa fa-flag"&gt;&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>h2 red</t>
   </si>
   <si>
     <t>r_improvement_areas</t>
@@ -904,6 +917,36 @@
   </si>
   <si>
     <t>selected(${follow_up_again}, "yes")</t>
+  </si>
+  <si>
+    <t>. &gt; today()</t>
+  </si>
+  <si>
+    <t>Date cannot be a past date or today</t>
+  </si>
+  <si>
+    <t>c_formatted_follow_up_date</t>
+  </si>
+  <si>
+    <t>format-date(${next_follow_up_date}, '%a %e %b %Y')</t>
+  </si>
+  <si>
+    <t>r_next_follow_up</t>
+  </si>
+  <si>
+    <t>Next follow up on **_${c_formatted_follow_up_date}_**.</t>
+  </si>
+  <si>
+    <t>c_formatted_task_date</t>
+  </si>
+  <si>
+    <t>format-date(date(decimal-date-time(${next_follow_up_date}) - 2), '%a %e %b %Y')</t>
+  </si>
+  <si>
+    <t>r_followup_note</t>
+  </si>
+  <si>
+    <t>A quality monitoring follow up task for ${chw_name} will appear on *_${c_formatted_task_date}_*.</t>
   </si>
   <si>
     <t>list_name</t>
@@ -1099,13 +1142,13 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
@@ -1345,7 +1388,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="10" width="18.0"/>
-    <col customWidth="1" min="11" max="11" width="72.25"/>
+    <col customWidth="1" min="11" max="11" width="71.75"/>
     <col customWidth="1" min="12" max="26" width="18.0"/>
   </cols>
   <sheetData>
@@ -5892,75 +5935,79 @@
       <c r="D130" s="10"/>
       <c r="E130" s="10"/>
       <c r="F130" s="10"/>
-      <c r="G130" s="10"/>
-      <c r="H130" s="10"/>
-      <c r="I130" s="10"/>
-      <c r="J130" s="10"/>
-      <c r="K130" s="10"/>
-      <c r="L130" s="10"/>
-      <c r="M130" s="10"/>
-      <c r="N130" s="10"/>
-      <c r="O130" s="10"/>
-      <c r="P130" s="10"/>
-      <c r="Q130" s="10"/>
-      <c r="R130" s="10"/>
-      <c r="S130" s="10"/>
-      <c r="T130" s="10"/>
-      <c r="U130" s="10"/>
-      <c r="V130" s="10"/>
-      <c r="W130" s="10"/>
-      <c r="X130" s="10"/>
-      <c r="Y130" s="10"/>
-      <c r="Z130" s="10"/>
+      <c r="G130" s="9" t="s">
+        <v>262</v>
+      </c>
+      <c r="H130" s="4"/>
+      <c r="I130" s="4"/>
+      <c r="J130" s="4"/>
+      <c r="K130" s="4"/>
+      <c r="L130" s="4"/>
+      <c r="M130" s="4"/>
+      <c r="N130" s="4"/>
+      <c r="O130" s="4"/>
+      <c r="P130" s="4"/>
+      <c r="Q130" s="4"/>
+      <c r="R130" s="4"/>
+      <c r="S130" s="4"/>
+      <c r="T130" s="4"/>
+      <c r="U130" s="4"/>
+      <c r="V130" s="4"/>
+      <c r="W130" s="4"/>
+      <c r="X130" s="4"/>
+      <c r="Y130" s="4"/>
+      <c r="Z130" s="4"/>
     </row>
     <row r="131">
-      <c r="A131" s="3" t="s">
+      <c r="A131" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="B131" s="3" t="s">
-        <v>262</v>
-      </c>
-      <c r="C131" s="3" t="s">
+      <c r="B131" s="9" t="s">
         <v>263</v>
       </c>
-      <c r="D131" s="4"/>
-      <c r="E131" s="4"/>
-      <c r="F131" s="4"/>
-      <c r="G131" s="4"/>
-      <c r="H131" s="4"/>
-      <c r="I131" s="4"/>
-      <c r="J131" s="4"/>
-      <c r="K131" s="4"/>
-      <c r="L131" s="4"/>
-      <c r="M131" s="4"/>
-      <c r="N131" s="4"/>
-      <c r="O131" s="4"/>
-      <c r="P131" s="4"/>
-      <c r="Q131" s="4"/>
-      <c r="R131" s="4"/>
-      <c r="S131" s="4"/>
-      <c r="T131" s="4"/>
-      <c r="U131" s="4"/>
-      <c r="V131" s="4"/>
-      <c r="W131" s="4"/>
-      <c r="X131" s="4"/>
-      <c r="Y131" s="4"/>
-      <c r="Z131" s="4"/>
+      <c r="C131" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="D131" s="10"/>
+      <c r="E131" s="10"/>
+      <c r="F131" s="10"/>
+      <c r="G131" s="10"/>
+      <c r="H131" s="10"/>
+      <c r="I131" s="10"/>
+      <c r="J131" s="10"/>
+      <c r="K131" s="10"/>
+      <c r="L131" s="10"/>
+      <c r="M131" s="10"/>
+      <c r="N131" s="10"/>
+      <c r="O131" s="10"/>
+      <c r="P131" s="10"/>
+      <c r="Q131" s="10"/>
+      <c r="R131" s="10"/>
+      <c r="S131" s="10"/>
+      <c r="T131" s="10"/>
+      <c r="U131" s="10"/>
+      <c r="V131" s="10"/>
+      <c r="W131" s="10"/>
+      <c r="X131" s="10"/>
+      <c r="Y131" s="10"/>
+      <c r="Z131" s="10"/>
     </row>
     <row r="132">
       <c r="A132" s="3" t="s">
         <v>44</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C132" s="3" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D132" s="4"/>
       <c r="E132" s="4"/>
       <c r="F132" s="4"/>
-      <c r="G132" s="4"/>
+      <c r="G132" s="3" t="s">
+        <v>267</v>
+      </c>
       <c r="H132" s="4"/>
       <c r="I132" s="4"/>
       <c r="J132" s="4"/>
@@ -5982,55 +6029,55 @@
       <c r="Z132" s="4"/>
     </row>
     <row r="133">
-      <c r="A133" s="9" t="s">
+      <c r="A133" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B133" s="9" t="s">
-        <v>266</v>
+      <c r="B133" s="3" t="s">
+        <v>268</v>
       </c>
-      <c r="C133" s="9" t="s">
+      <c r="C133" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="D133" s="4"/>
+      <c r="E133" s="4"/>
+      <c r="F133" s="4"/>
+      <c r="G133" s="4"/>
+      <c r="H133" s="4"/>
+      <c r="I133" s="4"/>
+      <c r="J133" s="4"/>
+      <c r="K133" s="4"/>
+      <c r="L133" s="4"/>
+      <c r="M133" s="4"/>
+      <c r="N133" s="4"/>
+      <c r="O133" s="4"/>
+      <c r="P133" s="4"/>
+      <c r="Q133" s="4"/>
+      <c r="R133" s="4"/>
+      <c r="S133" s="4"/>
+      <c r="T133" s="4"/>
+      <c r="U133" s="4"/>
+      <c r="V133" s="4"/>
+      <c r="W133" s="4"/>
+      <c r="X133" s="4"/>
+      <c r="Y133" s="4"/>
+      <c r="Z133" s="4"/>
+    </row>
+    <row r="134">
+      <c r="A134" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B134" s="9" t="s">
+        <v>270</v>
+      </c>
+      <c r="C134" s="9" t="s">
+        <v>271</v>
+      </c>
+      <c r="D134" s="10"/>
+      <c r="E134" s="10"/>
+      <c r="F134" s="10"/>
+      <c r="G134" s="11" t="s">
         <v>267</v>
       </c>
-      <c r="D133" s="10"/>
-      <c r="E133" s="10"/>
-      <c r="F133" s="10"/>
-      <c r="G133" s="10"/>
-      <c r="H133" s="10"/>
-      <c r="I133" s="10"/>
-      <c r="J133" s="10"/>
-      <c r="K133" s="10"/>
-      <c r="L133" s="10"/>
-      <c r="M133" s="10"/>
-      <c r="N133" s="10"/>
-      <c r="O133" s="10"/>
-      <c r="P133" s="10"/>
-      <c r="Q133" s="10"/>
-      <c r="R133" s="10"/>
-      <c r="S133" s="10"/>
-      <c r="T133" s="10"/>
-      <c r="U133" s="10"/>
-      <c r="V133" s="10"/>
-      <c r="W133" s="10"/>
-      <c r="X133" s="10"/>
-      <c r="Y133" s="10"/>
-      <c r="Z133" s="10"/>
-    </row>
-    <row r="134">
-      <c r="A134" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="B134" s="11" t="s">
-        <v>268</v>
-      </c>
-      <c r="C134" s="12" t="s">
-        <v>269</v>
-      </c>
-      <c r="D134" s="10"/>
-      <c r="E134" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="F134" s="10"/>
-      <c r="G134" s="10"/>
       <c r="H134" s="10"/>
       <c r="I134" s="10"/>
       <c r="J134" s="10"/>
@@ -6052,87 +6099,105 @@
       <c r="Z134" s="10"/>
     </row>
     <row r="135">
-      <c r="A135" s="11" t="s">
-        <v>270</v>
+      <c r="A135" s="9" t="s">
+        <v>54</v>
       </c>
-      <c r="B135" s="11" t="s">
-        <v>271</v>
-      </c>
-      <c r="C135" s="3" t="s">
+      <c r="B135" s="12" t="s">
         <v>272</v>
       </c>
-      <c r="D135" s="4"/>
-      <c r="E135" s="3" t="s">
+      <c r="C135" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="D135" s="10"/>
+      <c r="E135" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="F135" s="3" t="s">
-        <v>273</v>
+      <c r="F135" s="10"/>
+      <c r="G135" s="10"/>
+      <c r="H135" s="10"/>
+      <c r="I135" s="10"/>
+      <c r="J135" s="10"/>
+      <c r="K135" s="10"/>
+      <c r="L135" s="10"/>
+      <c r="M135" s="10"/>
+      <c r="N135" s="10"/>
+      <c r="O135" s="10"/>
+      <c r="P135" s="10"/>
+      <c r="Q135" s="10"/>
+      <c r="R135" s="10"/>
+      <c r="S135" s="10"/>
+      <c r="T135" s="10"/>
+      <c r="U135" s="10"/>
+      <c r="V135" s="10"/>
+      <c r="W135" s="10"/>
+      <c r="X135" s="10"/>
+      <c r="Y135" s="10"/>
+      <c r="Z135" s="10"/>
+    </row>
+    <row r="136">
+      <c r="A136" s="12" t="s">
+        <v>274</v>
       </c>
-      <c r="G135" s="4"/>
-      <c r="H135" s="4"/>
-      <c r="I135" s="4"/>
-      <c r="J135" s="4"/>
-      <c r="K135" s="4"/>
-      <c r="L135" s="4"/>
-      <c r="M135" s="4"/>
-      <c r="N135" s="4"/>
-      <c r="O135" s="4"/>
-      <c r="P135" s="4"/>
-      <c r="Q135" s="4"/>
-      <c r="R135" s="4"/>
-      <c r="S135" s="4"/>
-      <c r="T135" s="4"/>
-      <c r="U135" s="4"/>
-      <c r="V135" s="4"/>
-      <c r="W135" s="4"/>
-      <c r="X135" s="4"/>
-      <c r="Y135" s="4"/>
-      <c r="Z135" s="4"/>
-    </row>
-    <row r="136">
-      <c r="A136" s="9" t="s">
-        <v>35</v>
+      <c r="B136" s="12" t="s">
+        <v>275</v>
       </c>
-      <c r="B136" s="9" t="s">
-        <v>257</v>
+      <c r="C136" s="3" t="s">
+        <v>276</v>
       </c>
-      <c r="C136" s="10"/>
-      <c r="D136" s="10"/>
-      <c r="E136" s="10"/>
-      <c r="F136" s="10"/>
-      <c r="G136" s="10"/>
-      <c r="H136" s="10"/>
-      <c r="I136" s="10"/>
-      <c r="J136" s="10"/>
-      <c r="K136" s="10"/>
-      <c r="L136" s="10"/>
-      <c r="M136" s="10"/>
-      <c r="N136" s="10"/>
-      <c r="O136" s="10"/>
-      <c r="P136" s="10"/>
-      <c r="Q136" s="10"/>
-      <c r="R136" s="10"/>
-      <c r="S136" s="10"/>
-      <c r="T136" s="10"/>
-      <c r="U136" s="10"/>
-      <c r="V136" s="10"/>
-      <c r="W136" s="10"/>
-      <c r="X136" s="10"/>
-      <c r="Y136" s="10"/>
-      <c r="Z136" s="10"/>
+      <c r="D136" s="4"/>
+      <c r="E136" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F136" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="G136" s="4"/>
+      <c r="H136" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="I136" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="J136" s="4"/>
+      <c r="K136" s="4"/>
+      <c r="L136" s="4"/>
+      <c r="M136" s="4"/>
+      <c r="N136" s="4"/>
+      <c r="O136" s="4"/>
+      <c r="P136" s="4"/>
+      <c r="Q136" s="4"/>
+      <c r="R136" s="4"/>
+      <c r="S136" s="4"/>
+      <c r="T136" s="4"/>
+      <c r="U136" s="4"/>
+      <c r="V136" s="4"/>
+      <c r="W136" s="4"/>
+      <c r="X136" s="4"/>
+      <c r="Y136" s="4"/>
+      <c r="Z136" s="4"/>
     </row>
     <row r="137">
-      <c r="A137" s="4"/>
-      <c r="B137" s="4"/>
-      <c r="C137" s="4"/>
+      <c r="A137" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B137" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="C137" s="3" t="s">
+        <v>252</v>
+      </c>
       <c r="D137" s="4"/>
       <c r="E137" s="4"/>
-      <c r="F137" s="4"/>
+      <c r="F137" s="3" t="s">
+        <v>277</v>
+      </c>
       <c r="G137" s="4"/>
       <c r="H137" s="4"/>
       <c r="I137" s="4"/>
       <c r="J137" s="4"/>
-      <c r="K137" s="4"/>
+      <c r="K137" s="3" t="s">
+        <v>281</v>
+      </c>
       <c r="L137" s="4"/>
       <c r="M137" s="4"/>
       <c r="N137" s="4"/>
@@ -6150,12 +6215,20 @@
       <c r="Z137" s="4"/>
     </row>
     <row r="138">
-      <c r="A138" s="4"/>
-      <c r="B138" s="4"/>
-      <c r="C138" s="4"/>
+      <c r="A138" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B138" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="C138" s="3" t="s">
+        <v>283</v>
+      </c>
       <c r="D138" s="4"/>
       <c r="E138" s="4"/>
-      <c r="F138" s="4"/>
+      <c r="F138" s="3" t="s">
+        <v>277</v>
+      </c>
       <c r="G138" s="4"/>
       <c r="H138" s="4"/>
       <c r="I138" s="4"/>
@@ -6178,88 +6251,106 @@
       <c r="Z138" s="4"/>
     </row>
     <row r="139">
-      <c r="A139" s="4"/>
-      <c r="B139" s="4"/>
-      <c r="C139" s="4"/>
-      <c r="D139" s="4"/>
-      <c r="E139" s="4"/>
-      <c r="F139" s="4"/>
-      <c r="G139" s="4"/>
-      <c r="H139" s="4"/>
-      <c r="I139" s="4"/>
-      <c r="J139" s="4"/>
-      <c r="K139" s="4"/>
-      <c r="L139" s="4"/>
-      <c r="M139" s="4"/>
-      <c r="N139" s="4"/>
-      <c r="O139" s="4"/>
-      <c r="P139" s="4"/>
-      <c r="Q139" s="4"/>
-      <c r="R139" s="4"/>
-      <c r="S139" s="4"/>
-      <c r="T139" s="4"/>
-      <c r="U139" s="4"/>
-      <c r="V139" s="4"/>
-      <c r="W139" s="4"/>
-      <c r="X139" s="4"/>
-      <c r="Y139" s="4"/>
-      <c r="Z139" s="4"/>
+      <c r="A139" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B139" s="9" t="s">
+        <v>284</v>
+      </c>
+      <c r="C139" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="D139" s="10"/>
+      <c r="E139" s="10"/>
+      <c r="F139" s="10"/>
+      <c r="G139" s="10"/>
+      <c r="H139" s="10"/>
+      <c r="I139" s="10"/>
+      <c r="J139" s="10"/>
+      <c r="K139" s="13" t="s">
+        <v>285</v>
+      </c>
+      <c r="L139" s="10"/>
+      <c r="M139" s="10"/>
+      <c r="N139" s="10"/>
+      <c r="O139" s="10"/>
+      <c r="P139" s="10"/>
+      <c r="Q139" s="10"/>
+      <c r="R139" s="10"/>
+      <c r="S139" s="10"/>
+      <c r="T139" s="10"/>
+      <c r="U139" s="10"/>
+      <c r="V139" s="10"/>
+      <c r="W139" s="10"/>
+      <c r="X139" s="10"/>
+      <c r="Y139" s="10"/>
+      <c r="Z139" s="10"/>
     </row>
     <row r="140">
-      <c r="A140" s="4"/>
-      <c r="B140" s="4"/>
-      <c r="C140" s="4"/>
-      <c r="D140" s="4"/>
-      <c r="E140" s="4"/>
-      <c r="F140" s="4"/>
-      <c r="G140" s="4"/>
-      <c r="H140" s="4"/>
-      <c r="I140" s="4"/>
-      <c r="J140" s="4"/>
-      <c r="K140" s="4"/>
-      <c r="L140" s="4"/>
-      <c r="M140" s="4"/>
-      <c r="N140" s="4"/>
-      <c r="O140" s="4"/>
-      <c r="P140" s="4"/>
-      <c r="Q140" s="4"/>
-      <c r="R140" s="4"/>
-      <c r="S140" s="4"/>
-      <c r="T140" s="4"/>
-      <c r="U140" s="4"/>
-      <c r="V140" s="4"/>
-      <c r="W140" s="4"/>
-      <c r="X140" s="4"/>
-      <c r="Y140" s="4"/>
-      <c r="Z140" s="4"/>
+      <c r="A140" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B140" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="C140" s="13" t="s">
+        <v>287</v>
+      </c>
+      <c r="D140" s="10"/>
+      <c r="E140" s="10"/>
+      <c r="F140" s="10"/>
+      <c r="G140" s="10"/>
+      <c r="H140" s="10"/>
+      <c r="I140" s="10"/>
+      <c r="J140" s="10"/>
+      <c r="K140" s="10"/>
+      <c r="L140" s="10"/>
+      <c r="M140" s="10"/>
+      <c r="N140" s="10"/>
+      <c r="O140" s="10"/>
+      <c r="P140" s="10"/>
+      <c r="Q140" s="10"/>
+      <c r="R140" s="10"/>
+      <c r="S140" s="10"/>
+      <c r="T140" s="10"/>
+      <c r="U140" s="10"/>
+      <c r="V140" s="10"/>
+      <c r="W140" s="10"/>
+      <c r="X140" s="10"/>
+      <c r="Y140" s="10"/>
+      <c r="Z140" s="10"/>
     </row>
     <row r="141">
-      <c r="A141" s="4"/>
-      <c r="B141" s="4"/>
-      <c r="C141" s="4"/>
-      <c r="D141" s="4"/>
-      <c r="E141" s="4"/>
-      <c r="F141" s="4"/>
-      <c r="G141" s="4"/>
-      <c r="H141" s="4"/>
-      <c r="I141" s="4"/>
-      <c r="J141" s="4"/>
-      <c r="K141" s="4"/>
-      <c r="L141" s="4"/>
-      <c r="M141" s="4"/>
-      <c r="N141" s="4"/>
-      <c r="O141" s="4"/>
-      <c r="P141" s="4"/>
-      <c r="Q141" s="4"/>
-      <c r="R141" s="4"/>
-      <c r="S141" s="4"/>
-      <c r="T141" s="4"/>
-      <c r="U141" s="4"/>
-      <c r="V141" s="4"/>
-      <c r="W141" s="4"/>
-      <c r="X141" s="4"/>
-      <c r="Y141" s="4"/>
-      <c r="Z141" s="4"/>
+      <c r="A141" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B141" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="C141" s="10"/>
+      <c r="D141" s="10"/>
+      <c r="E141" s="10"/>
+      <c r="F141" s="10"/>
+      <c r="G141" s="10"/>
+      <c r="H141" s="10"/>
+      <c r="I141" s="10"/>
+      <c r="J141" s="10"/>
+      <c r="K141" s="10"/>
+      <c r="L141" s="10"/>
+      <c r="M141" s="10"/>
+      <c r="N141" s="10"/>
+      <c r="O141" s="10"/>
+      <c r="P141" s="10"/>
+      <c r="Q141" s="10"/>
+      <c r="R141" s="10"/>
+      <c r="S141" s="10"/>
+      <c r="T141" s="10"/>
+      <c r="U141" s="10"/>
+      <c r="V141" s="10"/>
+      <c r="W141" s="10"/>
+      <c r="X141" s="10"/>
+      <c r="Y141" s="10"/>
+      <c r="Z141" s="10"/>
     </row>
     <row r="142">
       <c r="A142" s="4"/>
@@ -30364,7 +30455,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="14" t="s">
-        <v>274</v>
+        <v>288</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>1</v>
@@ -30400,142 +30491,142 @@
     </row>
     <row r="2">
       <c r="A2" s="16" t="s">
-        <v>275</v>
+        <v>289</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>58</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>276</v>
+        <v>290</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>277</v>
+        <v>291</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="16" t="s">
-        <v>275</v>
+        <v>289</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>278</v>
+        <v>292</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>279</v>
+        <v>293</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>280</v>
+        <v>294</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="16" t="s">
-        <v>281</v>
+        <v>295</v>
       </c>
       <c r="B5" s="16" t="s">
         <v>58</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>276</v>
+        <v>290</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>277</v>
+        <v>291</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="16" t="s">
-        <v>281</v>
+        <v>295</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>278</v>
+        <v>292</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>279</v>
+        <v>293</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>280</v>
+        <v>294</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="16" t="s">
-        <v>281</v>
+        <v>295</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>282</v>
+        <v>296</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>283</v>
+        <v>297</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>284</v>
+        <v>298</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="16" t="s">
-        <v>285</v>
+        <v>299</v>
       </c>
       <c r="B9" s="16">
         <v>0.0</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>286</v>
+        <v>300</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>287</v>
+        <v>301</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="16" t="s">
-        <v>285</v>
+        <v>299</v>
       </c>
       <c r="B10" s="16">
         <v>1.0</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>288</v>
+        <v>302</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>289</v>
+        <v>303</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="16" t="s">
-        <v>285</v>
+        <v>299</v>
       </c>
       <c r="B11" s="16">
         <v>2.0</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>290</v>
+        <v>304</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>291</v>
+        <v>305</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="16" t="s">
-        <v>285</v>
+        <v>299</v>
       </c>
       <c r="B12" s="16">
         <v>3.0</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>292</v>
+        <v>306</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>293</v>
+        <v>307</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="16" t="s">
-        <v>285</v>
+        <v>299</v>
       </c>
       <c r="B13" s="16">
         <v>5.0</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>294</v>
+        <v>308</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>295</v>
+        <v>309</v>
       </c>
     </row>
     <row r="15">
@@ -30543,13 +30634,13 @@
         <v>222</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>296</v>
+        <v>310</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>297</v>
+        <v>311</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>298</v>
+        <v>312</v>
       </c>
     </row>
     <row r="16">
@@ -30557,13 +30648,13 @@
         <v>222</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>299</v>
+        <v>313</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>300</v>
+        <v>314</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>301</v>
+        <v>315</v>
       </c>
     </row>
   </sheetData>
@@ -30589,22 +30680,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>302</v>
+        <v>316</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>303</v>
+        <v>317</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>304</v>
+        <v>318</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>305</v>
+        <v>319</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>306</v>
+        <v>320</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>307</v>
+        <v>321</v>
       </c>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
@@ -30632,20 +30723,20 @@
         <v>212</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>308</v>
+        <v>322</v>
       </c>
       <c r="C2" s="17">
         <f>NOW()</f>
-        <v>44741.60844</v>
+        <v>44746.42615</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>309</v>
+        <v>323</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>310</v>
+        <v>324</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>311</v>
+        <v>325</v>
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>

</xml_diff>